<commit_message>
Création de nx mappings 0e3f71524d31ae38b8fd94d7fa5f14a19c184959
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/FRDeviceRequestLMCDAFHIR.xlsx
+++ b/mappingCorps/ig/FRDeviceRequestLMCDAFHIR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Property</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-29T15:05:54+00:00</t>
+    <t>2026-01-05T15:47:03+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -139,6 +139,36 @@
     <t>FRCDADispositifMedical.effectiveTime</t>
   </si>
   <si>
+    <t>FRLMDispositifMedicalEntree.renouvellement</t>
+  </si>
+  <si>
+    <t>FRCDADispositifMedical.repeatNumber</t>
+  </si>
+  <si>
+    <t>FRLMDispositifMedicalEntree.duree</t>
+  </si>
+  <si>
+    <t>FRCDADispositifMedical.expectedUseTime</t>
+  </si>
+  <si>
+    <t>FRLMDispositifMedicalEntree.quantite</t>
+  </si>
+  <si>
+    <t>FRCDADispositifMedical.quantity</t>
+  </si>
+  <si>
+    <t>FRLMDispositifMedicalEntree.auteur</t>
+  </si>
+  <si>
+    <t>FRCDADispositifMedical.author</t>
+  </si>
+  <si>
+    <t>FRLMDispositifMedicalEntree.dispositifMedical</t>
+  </si>
+  <si>
+    <t>FRCDADispositifMedical.participant</t>
+  </si>
+  <si>
     <t>FRLMDispositifMedicalEntree.affectionLongueDuree</t>
   </si>
   <si>
@@ -175,34 +205,19 @@
     <t>FRDeviceRequestDocument.note</t>
   </si>
   <si>
-    <t>FRDeviceRequestDocument.occurrenceTiming</t>
-  </si>
-  <si>
-    <t>FRCDADispositifMedical.repeatNumber</t>
+    <t>FRDeviceRequestDocument.occurrence[x]</t>
   </si>
   <si>
     <t>FRDeviceRequestDocument.occurrenceTiming.repeat.count</t>
   </si>
   <si>
-    <t>FRCDADispositifMedical.expectedUseTime</t>
-  </si>
-  <si>
     <t>FRDeviceRequestDocument.occurrencePeriod</t>
   </si>
   <si>
-    <t>FRCDADispositifMedical.quantity</t>
-  </si>
-  <si>
     <t>FRDeviceRequestDocument.parameter.valueQuantity</t>
   </si>
   <si>
-    <t>FRCDADispositifMedical.author</t>
-  </si>
-  <si>
     <t>FRDeviceRequestDocument.requester.extension.prescripteur</t>
-  </si>
-  <si>
-    <t>FRCDADispositifMedical.participant</t>
   </si>
   <si>
     <t>FRDeviceRequestDocument.codeReference</t>
@@ -474,7 +489,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -617,6 +632,71 @@
         <v>48</v>
       </c>
       <c r="E10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -659,7 +739,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>30</v>
@@ -674,7 +754,7 @@
         <v>33</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -687,7 +767,7 @@
         <v>33</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -700,7 +780,7 @@
         <v>33</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -713,124 +793,124 @@
         <v>33</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E15" s="2"/>
     </row>

</xml_diff>